<commit_message>
modification of predictions file
</commit_message>
<xml_diff>
--- a/dat/predictions.xlsx
+++ b/dat/predictions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anama\Desktop\appClimate\dat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0F61FEBA-843B-4FBE-A0F1-70CA99B64C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{56CCA3A8-2C98-4124-AF9F-1DBAD4C2EC42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25693" yWindow="-3913" windowWidth="25786" windowHeight="13866"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="21">
   <si>
     <t>Austria</t>
   </si>
@@ -64,28 +64,16 @@
     <t>Hungary</t>
   </si>
   <si>
-    <t xml:space="preserve">  97.8723078 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  99.34396257</t>
-  </si>
-  <si>
     <t>Italy</t>
   </si>
   <si>
     <t>Portugal</t>
   </si>
   <si>
-    <t xml:space="preserve">  98.45190365</t>
-  </si>
-  <si>
     <t>Romania</t>
   </si>
   <si>
     <t>Spain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  96.98718909</t>
   </si>
   <si>
     <t>Switzerland</t>
@@ -101,7 +89,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,6 +220,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -578,8 +574,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -935,1154 +932,756 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="4" width="11.42578125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1">
-        <v>2017</v>
-      </c>
-      <c r="D1">
-        <v>2018</v>
-      </c>
-      <c r="E1">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>100.91365635</v>
-      </c>
-      <c r="D2">
-        <v>101.13386515000001</v>
-      </c>
-      <c r="E2">
+      <c r="C2" s="1">
         <v>100.78390561000001</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>96.317926689999993</v>
-      </c>
-      <c r="D3">
-        <v>97.830186639999994</v>
-      </c>
-      <c r="E3">
+      <c r="C3" s="1">
         <v>98.106370490000003</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>100.27643157</v>
-      </c>
-      <c r="D4">
-        <v>100.27695131</v>
-      </c>
-      <c r="E4">
+      <c r="C4" s="1">
         <v>100.26647226999999</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5">
-        <v>100.40880244</v>
-      </c>
-      <c r="D5">
-        <v>100.37020252000001</v>
-      </c>
-      <c r="E5">
+      <c r="C5" s="1">
         <v>100.56273312</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6">
-        <v>100.18431889</v>
-      </c>
-      <c r="D6">
-        <v>102.18557177</v>
-      </c>
-      <c r="E6">
+      <c r="C6" s="1">
         <v>103.06658888</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C7">
-        <v>136.08600938999999</v>
-      </c>
-      <c r="D7">
-        <v>138.6511653</v>
-      </c>
-      <c r="E7">
+      <c r="C7" s="1">
         <v>144.69204912000001</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
       </c>
-      <c r="C8">
-        <v>82.278436029999995</v>
-      </c>
-      <c r="D8">
-        <v>82.644326469999996</v>
-      </c>
-      <c r="E8">
+      <c r="C8" s="1">
         <v>82.935228010000003</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
       </c>
-      <c r="C9">
-        <v>80.382770699999995</v>
-      </c>
-      <c r="D9">
-        <v>90.022256900000002</v>
-      </c>
-      <c r="E9">
+      <c r="C9" s="1">
         <v>88.263282380000007</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
-      <c r="C10">
-        <v>86.489149639999994</v>
-      </c>
-      <c r="D10">
-        <v>88.352953200000002</v>
-      </c>
-      <c r="E10">
+      <c r="C10" s="1">
         <v>89.113997780000005</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
       </c>
-      <c r="C11">
-        <v>125.20075713</v>
-      </c>
-      <c r="D11">
-        <v>122.95372281</v>
-      </c>
-      <c r="E11">
+      <c r="C11" s="1">
         <v>122.10701379</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
-      <c r="C12">
-        <v>107.01725978</v>
-      </c>
-      <c r="D12">
-        <v>106.26059102000001</v>
-      </c>
-      <c r="E12">
+      <c r="C12" s="1">
         <v>104.45998065000001</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
-      <c r="C13">
-        <v>106.74976873</v>
-      </c>
-      <c r="D13">
-        <v>105.11049342</v>
-      </c>
-      <c r="E13">
+      <c r="C13" s="1">
         <v>106.06718331</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
       </c>
-      <c r="C14">
-        <v>102.31680867</v>
-      </c>
-      <c r="D14">
-        <v>102.65796340999999</v>
-      </c>
-      <c r="E14">
+      <c r="C14" s="1">
         <v>101.41032549000001</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
       </c>
-      <c r="C15">
-        <v>100.62862841</v>
-      </c>
-      <c r="D15">
-        <v>102.43210446000001</v>
-      </c>
-      <c r="E15">
+      <c r="C15" s="1">
         <v>106.01826339</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
       </c>
-      <c r="C16">
-        <v>104.27749631</v>
-      </c>
-      <c r="D16">
-        <v>104.5508468</v>
-      </c>
-      <c r="E16">
+      <c r="C16" s="1">
         <v>101.74114513000001</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
       </c>
-      <c r="C17">
-        <v>100.49038739</v>
-      </c>
-      <c r="D17">
-        <v>100.46587728999999</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="C17" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
       </c>
-      <c r="C18">
-        <v>100.25401024</v>
-      </c>
-      <c r="D18">
-        <v>100.36874155</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="C18" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
       </c>
-      <c r="C19">
-        <v>104.76557506</v>
-      </c>
-      <c r="D19">
-        <v>104.67681992999999</v>
-      </c>
-      <c r="E19">
+      <c r="C19" s="1">
         <v>101.06183621</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
       <c r="B20" t="s">
         <v>1</v>
       </c>
-      <c r="C20">
-        <v>96.680248879999994</v>
-      </c>
-      <c r="D20">
-        <v>98.182633359999997</v>
-      </c>
-      <c r="E20">
+      <c r="C20" s="1">
         <v>98.64038961</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
       <c r="B21" t="s">
         <v>2</v>
       </c>
-      <c r="C21">
-        <v>88.76158144</v>
-      </c>
-      <c r="D21">
-        <v>92.745778430000001</v>
-      </c>
-      <c r="E21">
+      <c r="C21" s="1">
         <v>95.290419610000001</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
       </c>
-      <c r="C22">
-        <v>96.361617249999995</v>
-      </c>
-      <c r="D22">
-        <v>99.517692929999995</v>
-      </c>
-      <c r="E22">
+      <c r="C22" s="1">
         <v>99.590859929999993</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>11</v>
       </c>
       <c r="B23" t="s">
         <v>4</v>
       </c>
-      <c r="C23">
-        <v>97.308155510000006</v>
-      </c>
-      <c r="D23">
-        <v>98.543964939999995</v>
-      </c>
-      <c r="E23">
+      <c r="C23" s="1">
         <v>99.805857810000006</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>11</v>
       </c>
       <c r="B24" t="s">
         <v>5</v>
       </c>
-      <c r="C24">
-        <v>94.844258440000004</v>
-      </c>
-      <c r="D24">
-        <v>96.366968499999999</v>
-      </c>
-      <c r="E24">
+      <c r="C24" s="1">
         <v>97.86124332</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>11</v>
       </c>
       <c r="B25" t="s">
         <v>6</v>
       </c>
-      <c r="C25">
-        <v>98.472195959999993</v>
-      </c>
-      <c r="D25">
-        <v>96.604116599999998</v>
-      </c>
-      <c r="E25">
+      <c r="C25" s="1">
         <v>96.77865104</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>12</v>
       </c>
       <c r="B26" t="s">
         <v>1</v>
       </c>
-      <c r="C26">
-        <v>98.139208740000001</v>
-      </c>
-      <c r="D26">
-        <v>97.765718120000003</v>
-      </c>
-      <c r="E26">
+      <c r="C26" s="1">
         <v>98.984015470000003</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
       <c r="B27" t="s">
         <v>2</v>
       </c>
-      <c r="C27">
-        <v>111.1442412</v>
-      </c>
-      <c r="D27">
-        <v>110.04353057</v>
-      </c>
-      <c r="E27">
+      <c r="C27" s="1">
         <v>109.07637606999999</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
       </c>
-      <c r="C28">
-        <v>98.431645579999994</v>
-      </c>
-      <c r="D28">
-        <v>98.195899760000003</v>
-      </c>
-      <c r="E28">
+      <c r="C28" s="1">
         <v>98.417577840000007</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
       <c r="B29" t="s">
         <v>4</v>
       </c>
-      <c r="C29">
-        <v>106.6564657</v>
-      </c>
-      <c r="D29">
-        <v>106.21248224</v>
-      </c>
-      <c r="E29">
+      <c r="C29" s="1">
         <v>105.62910563</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
       <c r="B30" t="s">
         <v>5</v>
       </c>
-      <c r="C30">
-        <v>101.18918327999999</v>
-      </c>
-      <c r="D30">
-        <v>101.80659701</v>
-      </c>
-      <c r="E30">
+      <c r="C30" s="1">
         <v>101.58487408000001</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>12</v>
       </c>
       <c r="B31" t="s">
         <v>6</v>
       </c>
-      <c r="C31">
-        <v>96.955320459999996</v>
-      </c>
-      <c r="D31">
-        <v>95.829633709999996</v>
-      </c>
-      <c r="E31">
+      <c r="C31" s="1">
         <v>97.010018610000003</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>13</v>
       </c>
       <c r="B32" t="s">
         <v>1</v>
       </c>
-      <c r="C32">
-        <v>93.586704589999997</v>
-      </c>
-      <c r="D32" t="s">
-        <v>14</v>
-      </c>
-      <c r="E32">
+      <c r="C32" s="1">
         <v>100.21693777</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>13</v>
       </c>
       <c r="B33" t="s">
         <v>2</v>
       </c>
-      <c r="C33">
-        <v>82.471487420000003</v>
-      </c>
-      <c r="D33">
-        <v>90.642663810000002</v>
-      </c>
-      <c r="E33">
+      <c r="C33" s="1">
         <v>94.103178260000007</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>13</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
       </c>
-      <c r="C34">
-        <v>86.125632330000002</v>
-      </c>
-      <c r="D34">
-        <v>87.467533590000002</v>
-      </c>
-      <c r="E34">
+      <c r="C34" s="1">
         <v>88.287749649999995</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>13</v>
       </c>
       <c r="B35" t="s">
         <v>4</v>
       </c>
-      <c r="C35">
-        <v>102.32805860000001</v>
-      </c>
-      <c r="D35">
-        <v>103.29839664000001</v>
-      </c>
-      <c r="E35">
+      <c r="C35" s="1">
         <v>105.05666965</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>13</v>
       </c>
       <c r="B36" t="s">
         <v>5</v>
       </c>
-      <c r="C36">
-        <v>96.521144390000003</v>
-      </c>
-      <c r="D36">
-        <v>97.876180050000002</v>
-      </c>
-      <c r="E36">
+      <c r="C36" s="1">
         <v>99.081329940000003</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>13</v>
       </c>
       <c r="B37" t="s">
         <v>6</v>
       </c>
-      <c r="C37">
-        <v>96.400036779999994</v>
-      </c>
-      <c r="D37" t="s">
-        <v>15</v>
-      </c>
-      <c r="E37">
+      <c r="C37" s="1">
         <v>100.49915095</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B38" t="s">
         <v>1</v>
       </c>
-      <c r="C38">
-        <v>114.76766692</v>
-      </c>
-      <c r="D38">
-        <v>114.98633427</v>
-      </c>
-      <c r="E38">
+      <c r="C38" s="1">
         <v>115.42988078</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B39" t="s">
         <v>2</v>
       </c>
-      <c r="C39">
-        <v>106.0891984</v>
-      </c>
-      <c r="D39">
-        <v>106.31426761</v>
-      </c>
-      <c r="E39">
+      <c r="C39" s="1">
         <v>106.90631207</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B40" t="s">
         <v>3</v>
       </c>
-      <c r="C40">
-        <v>116.21616339000001</v>
-      </c>
-      <c r="D40">
-        <v>116.21311208</v>
-      </c>
-      <c r="E40">
+      <c r="C40" s="1">
         <v>117.26773403</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B41" t="s">
         <v>4</v>
       </c>
-      <c r="C41">
-        <v>110.88009538</v>
-      </c>
-      <c r="D41">
-        <v>110.41357401</v>
-      </c>
-      <c r="E41">
+      <c r="C41" s="1">
         <v>110.38771514</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B42" t="s">
         <v>5</v>
       </c>
-      <c r="C42">
-        <v>99.886886099999998</v>
-      </c>
-      <c r="D42">
-        <v>100.72507446</v>
-      </c>
-      <c r="E42">
+      <c r="C42" s="1">
         <v>102.59364644999999</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B43" t="s">
         <v>6</v>
       </c>
-      <c r="C43">
-        <v>111.59532879</v>
-      </c>
-      <c r="D43">
-        <v>111.31552096999999</v>
-      </c>
-      <c r="E43">
+      <c r="C43" s="1">
         <v>112.55965358</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B44" t="s">
         <v>1</v>
       </c>
-      <c r="C44">
-        <v>93.078343259999997</v>
-      </c>
-      <c r="D44">
-        <v>93.318639540000007</v>
-      </c>
-      <c r="E44">
+      <c r="C44" s="1">
         <v>95.01939093</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B45" t="s">
         <v>2</v>
       </c>
-      <c r="C45">
-        <v>93.759893070000004</v>
-      </c>
-      <c r="D45" t="s">
-        <v>18</v>
-      </c>
-      <c r="E45">
+      <c r="C45" s="1">
         <v>100.40655869</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B46" t="s">
         <v>3</v>
       </c>
-      <c r="C46">
-        <v>92.802395540000006</v>
-      </c>
-      <c r="D46">
-        <v>92.893648880000001</v>
-      </c>
-      <c r="E46">
+      <c r="C46" s="1">
         <v>94.044341579999994</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B47" t="s">
         <v>4</v>
       </c>
-      <c r="C47">
-        <v>96.407686609999999</v>
-      </c>
-      <c r="D47">
-        <v>96.155475139999993</v>
-      </c>
-      <c r="E47">
+      <c r="C47" s="1">
         <v>95.274115640000005</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B48" t="s">
         <v>5</v>
       </c>
-      <c r="C48">
-        <v>95.693750010000002</v>
-      </c>
-      <c r="D48">
-        <v>95.230676799999998</v>
-      </c>
-      <c r="E48">
+      <c r="C48" s="1">
         <v>99.066728929999996</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B49" t="s">
         <v>6</v>
       </c>
-      <c r="C49">
-        <v>89.403884050000002</v>
-      </c>
-      <c r="D49">
-        <v>89.668171979999997</v>
-      </c>
-      <c r="E49">
+      <c r="C49" s="1">
         <v>91.345064789999995</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B50" t="s">
         <v>1</v>
       </c>
-      <c r="C50">
-        <v>93.564523019999996</v>
-      </c>
-      <c r="D50">
-        <v>94.898291490000005</v>
-      </c>
-      <c r="E50">
+      <c r="C50" s="1">
         <v>98.114042560000001</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B51" t="s">
         <v>2</v>
       </c>
-      <c r="C51">
-        <v>83.732501869999993</v>
-      </c>
-      <c r="D51">
-        <v>86.281111469999999</v>
-      </c>
-      <c r="E51">
+      <c r="C51" s="1">
         <v>92.616519870000005</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B52" t="s">
         <v>3</v>
       </c>
-      <c r="C52">
-        <v>92.226781239999994</v>
-      </c>
-      <c r="D52">
-        <v>98.1965735</v>
-      </c>
-      <c r="E52">
+      <c r="C52" s="1">
         <v>98.539967559999994</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B53" t="s">
         <v>4</v>
       </c>
-      <c r="C53">
-        <v>101.69245761000001</v>
-      </c>
-      <c r="D53">
-        <v>102.00321580000001</v>
-      </c>
-      <c r="E53">
+      <c r="C53" s="1">
         <v>102.85358642</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B54" t="s">
         <v>5</v>
       </c>
-      <c r="C54">
-        <v>90.664917810000006</v>
-      </c>
-      <c r="D54">
-        <v>92.218591450000005</v>
-      </c>
-      <c r="E54">
+      <c r="C54" s="1">
         <v>93.681126329999998</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B55" t="s">
         <v>6</v>
       </c>
-      <c r="C55">
-        <v>106.59733014</v>
-      </c>
-      <c r="D55">
-        <v>107.14934201</v>
-      </c>
-      <c r="E55">
+      <c r="C55" s="1">
         <v>107.5758297</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B56" t="s">
         <v>1</v>
       </c>
-      <c r="C56">
-        <v>93.837949399999999</v>
-      </c>
-      <c r="D56" t="s">
-        <v>21</v>
-      </c>
-      <c r="E56">
+      <c r="C56" s="1">
         <v>100.9059002</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B57" t="s">
         <v>2</v>
       </c>
-      <c r="C57">
-        <v>96.845087289999995</v>
-      </c>
-      <c r="D57">
-        <v>101.70272312</v>
-      </c>
-      <c r="E57">
+      <c r="C57" s="1">
         <v>105.1490811</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B58" t="s">
         <v>3</v>
       </c>
-      <c r="C58">
-        <v>93.194402909999994</v>
-      </c>
-      <c r="D58">
-        <v>96.399362620000005</v>
-      </c>
-      <c r="E58">
+      <c r="C58" s="1">
         <v>99.865123769999997</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B59" t="s">
         <v>4</v>
       </c>
-      <c r="C59">
-        <v>91.666451679999994</v>
-      </c>
-      <c r="D59">
-        <v>92.513458940000007</v>
-      </c>
-      <c r="E59">
+      <c r="C59" s="1">
         <v>98.455877340000001</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B60" t="s">
         <v>5</v>
       </c>
-      <c r="C60">
-        <v>97.333510669999995</v>
-      </c>
-      <c r="D60">
-        <v>98.145316399999999</v>
-      </c>
-      <c r="E60">
+      <c r="C60" s="1">
         <v>99.422469169999999</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B61" t="s">
         <v>6</v>
       </c>
-      <c r="C61">
-        <v>89.773951479999994</v>
-      </c>
-      <c r="D61">
-        <v>93.972946030000003</v>
-      </c>
-      <c r="E61">
+      <c r="C61" s="1">
         <v>94.729901440000006</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B62" t="s">
         <v>1</v>
       </c>
-      <c r="C62">
-        <v>103.28681933</v>
-      </c>
-      <c r="D62">
-        <v>103.33007985</v>
-      </c>
-      <c r="E62">
+      <c r="C62" s="1">
         <v>101.93425827999999</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B63" t="s">
         <v>2</v>
       </c>
-      <c r="C63">
-        <v>134.56683028</v>
-      </c>
-      <c r="D63">
-        <v>138.53950209000001</v>
-      </c>
-      <c r="E63">
+      <c r="C63" s="1">
         <v>136.27264557000001</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B64" t="s">
         <v>3</v>
       </c>
-      <c r="C64">
-        <v>105.38906726</v>
-      </c>
-      <c r="D64">
-        <v>105.80337517</v>
-      </c>
-      <c r="E64">
+      <c r="C64" s="1">
         <v>105.25731621</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B65" t="s">
         <v>4</v>
       </c>
-      <c r="C65">
-        <v>103.00038837</v>
-      </c>
-      <c r="D65">
-        <v>103.10998609000001</v>
-      </c>
-      <c r="E65">
+      <c r="C65" s="1">
         <v>101.87351374000001</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B66" t="s">
         <v>5</v>
       </c>
-      <c r="C66">
-        <v>106.96756868</v>
-      </c>
-      <c r="D66">
-        <v>106.95629018</v>
-      </c>
-      <c r="E66">
+      <c r="C66" s="1">
         <v>106.50433221</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B67" t="s">
         <v>6</v>
       </c>
-      <c r="C67">
-        <v>113.47991695</v>
-      </c>
-      <c r="D67">
-        <v>113.34519708000001</v>
-      </c>
-      <c r="E67">
+      <c r="C67" s="1">
         <v>112.61904783</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>